<commit_message>
Executed and documented from_itemis tests
</commit_message>
<xml_diff>
--- a/doc/TestResults.xlsx
+++ b/doc/TestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\ProgettiGit\test-generator-for-yakindu\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3A2C0C-B378-48CB-A309-382D89CA457E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2C2155-0ED8-414E-9744-558185846842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{95FB7F74-23E6-4942-9272-C4518354FDE6}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15024" windowHeight="12336" xr2:uid="{95FB7F74-23E6-4942-9272-C4518354FDE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="157">
   <si>
     <t>Cartella</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t xml:space="preserve">ERRORS </t>
+  </si>
+  <si>
+    <t>FAIELD</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -701,8 +704,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -720,9 +721,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -744,6 +742,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1079,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B27DDD8-03C6-4820-BB99-CEA8F91EE15F}">
-  <dimension ref="A1:H139"/>
+  <dimension ref="A1:Q139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L125" sqref="L125"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,23 +1105,23 @@
     <col min="1" max="1" width="44.44140625" customWidth="1"/>
     <col min="2" max="2" width="49.88671875" customWidth="1"/>
     <col min="3" max="8" width="22.21875" customWidth="1"/>
-    <col min="12" max="12" width="68.6640625" customWidth="1"/>
+    <col min="12" max="12" width="45.44140625" customWidth="1"/>
     <col min="13" max="13" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="27" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1118,16 +1133,16 @@
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="21" t="s">
         <v>152</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="21" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="8" t="s">
@@ -1141,12 +1156,12 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1155,12 +1170,12 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1169,12 +1184,12 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1183,12 +1198,12 @@
       <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="17"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1197,12 +1212,12 @@
       <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1211,12 +1226,12 @@
       <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="17"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1225,12 +1240,12 @@
       <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1239,12 +1254,12 @@
       <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="17"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1253,12 +1268,12 @@
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1267,12 +1282,12 @@
       <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1281,12 +1296,12 @@
       <c r="B13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1295,12 +1310,12 @@
       <c r="B14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1309,12 +1324,12 @@
       <c r="B15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1323,14 +1338,14 @@
       <c r="B16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1338,13 +1353,13 @@
         <v>29</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="26"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="12"/>
       <c r="F17" s="9"/>
       <c r="G17" s="12"/>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -1352,13 +1367,13 @@
         <v>30</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="26"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="12"/>
       <c r="F18" s="9"/>
       <c r="G18" s="12"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1366,13 +1381,13 @@
         <v>31</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="26"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="12"/>
       <c r="F19" s="9"/>
       <c r="G19" s="12"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1380,13 +1395,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="26"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="12"/>
       <c r="F20" s="9"/>
       <c r="G20" s="12"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1394,13 +1409,13 @@
         <v>33</v>
       </c>
       <c r="C21" s="10"/>
-      <c r="D21" s="26"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="12"/>
       <c r="F21" s="9"/>
       <c r="G21" s="12"/>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1408,13 +1423,13 @@
         <v>34</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="26"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="12"/>
       <c r="F22" s="9"/>
       <c r="G22" s="12"/>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1422,13 +1437,13 @@
         <v>35</v>
       </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="26"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="12"/>
       <c r="F23" s="9"/>
       <c r="G23" s="12"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -1436,13 +1451,13 @@
         <v>36</v>
       </c>
       <c r="C24" s="10"/>
-      <c r="D24" s="26"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="12"/>
       <c r="F24" s="9"/>
       <c r="G24" s="12"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -1450,13 +1465,13 @@
         <v>37</v>
       </c>
       <c r="C25" s="10"/>
-      <c r="D25" s="26"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="12"/>
       <c r="F25" s="9"/>
       <c r="G25" s="12"/>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1464,13 +1479,13 @@
         <v>38</v>
       </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="26"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="12"/>
       <c r="F26" s="9"/>
       <c r="G26" s="12"/>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1478,13 +1493,13 @@
         <v>39</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="26"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="12"/>
       <c r="F27" s="9"/>
       <c r="G27" s="12"/>
       <c r="H27" s="11"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
@@ -1492,13 +1507,13 @@
         <v>40</v>
       </c>
       <c r="C28" s="10"/>
-      <c r="D28" s="26"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="12"/>
       <c r="F28" s="9"/>
       <c r="G28" s="12"/>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1512,7 +1527,7 @@
       <c r="G29" s="12"/>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1526,7 +1541,7 @@
       <c r="G30" s="12"/>
       <c r="H30" s="11"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1539,1046 +1554,1791 @@
       <c r="F31" s="9"/>
       <c r="G31" s="12"/>
       <c r="H31" s="11"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L31" s="27"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="14"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C32" s="29">
+        <v>0.63176248711678296</v>
+      </c>
+      <c r="D32" s="33">
+        <v>0</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="F32" s="33">
+        <v>0.85562416453229095</v>
+      </c>
+      <c r="G32" s="18">
+        <v>0.82</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="L32" s="27"/>
+      <c r="Q32" s="27"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="11"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C33" s="28">
+        <v>0.64647567169069398</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" s="14">
+        <v>0</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="L33" s="27"/>
+      <c r="Q33" s="27"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C34" s="28">
+        <v>0.55820414642724903</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" s="28">
+        <v>0.69448534364233006</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0.35</v>
+      </c>
+      <c r="H34" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L34" s="27"/>
+      <c r="Q34" s="27"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="11"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C35" s="28">
+        <v>0.96208003952569099</v>
+      </c>
+      <c r="D35" s="12">
+        <v>1</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F35" s="28">
+        <v>0.92792373866542599</v>
+      </c>
+      <c r="G35" s="12">
+        <v>1</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L35" s="27"/>
+      <c r="Q35" s="27"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="11"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C36" s="28">
+        <v>0.61547016278488997</v>
+      </c>
+      <c r="D36" s="12">
+        <v>0</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F36" s="28">
+        <v>0.89887687359544699</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="L36" s="27"/>
+      <c r="Q36" s="27"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="11"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C37" s="28">
+        <v>0.97017663043478197</v>
+      </c>
+      <c r="D37" s="12">
+        <v>0.83</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F37" s="28">
+        <v>0.931858409124519</v>
+      </c>
+      <c r="G37" s="12">
+        <v>1</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L37" s="27"/>
+      <c r="Q37" s="27"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="11"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C38" s="28">
+        <v>0.631794019933554</v>
+      </c>
+      <c r="D38" s="12">
+        <v>0</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="28">
+        <v>0.933013565891472</v>
+      </c>
+      <c r="G38" s="12">
+        <v>1</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L38" s="27"/>
+      <c r="Q38" s="27"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C39" s="28">
+        <v>0.710413479950598</v>
+      </c>
+      <c r="D39" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="28">
+        <v>0.75699835332862797</v>
+      </c>
+      <c r="G39" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="H39" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L39" s="27"/>
+      <c r="Q39" s="27"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="11"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C40" s="28">
+        <v>0.969948107448107</v>
+      </c>
+      <c r="D40" s="12">
+        <v>1</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F40" s="28">
+        <v>0.93100368898241204</v>
+      </c>
+      <c r="G40" s="12">
+        <v>1</v>
+      </c>
+      <c r="H40" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L40" s="27"/>
+      <c r="Q40" s="27"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="11"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C41" s="28">
+        <v>0.60839404839600497</v>
+      </c>
+      <c r="D41" s="30">
+        <v>0</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="F41" s="28">
+        <v>0.84226745919726398</v>
+      </c>
+      <c r="G41" s="12">
+        <v>0.59</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L41" s="27"/>
+      <c r="Q41" s="27"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="11"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C42" s="28">
+        <v>0.59065144628566402</v>
+      </c>
+      <c r="D42" s="12">
+        <v>0</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="28">
+        <v>0.70955626646277004</v>
+      </c>
+      <c r="G42" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L42" s="27"/>
+      <c r="Q42" s="27"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="11"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C43" s="28">
+        <v>0.60349202498759502</v>
+      </c>
+      <c r="D43" s="12">
+        <v>0</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F43" s="28">
+        <v>0.73188083405662496</v>
+      </c>
+      <c r="G43" s="12">
+        <v>0.37</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L43" s="27"/>
+      <c r="Q43" s="27"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="11"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C44" s="28">
+        <v>0.97313823857302095</v>
+      </c>
+      <c r="D44" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F44" s="28">
+        <v>0.90745025792188605</v>
+      </c>
+      <c r="G44" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="H44" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L44" s="27"/>
+      <c r="Q44" s="27"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C45" s="28">
+        <v>0.58073920077125796</v>
+      </c>
+      <c r="D45" s="12">
+        <v>0</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F45" s="28">
+        <v>0.85603498968302505</v>
+      </c>
+      <c r="G45" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L45" s="27"/>
+      <c r="Q45" s="27"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="11"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C46" s="28">
+        <v>0.57412617958654499</v>
+      </c>
+      <c r="D46" s="12">
+        <v>0</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F46" s="28">
+        <v>0.83861853221988203</v>
+      </c>
+      <c r="G46" s="12">
+        <v>0.73</v>
+      </c>
+      <c r="H46" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L46" s="27"/>
+      <c r="Q46" s="27"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="11"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C47" s="28">
+        <v>0.54552514788675199</v>
+      </c>
+      <c r="D47" s="12">
+        <v>0</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F47" s="28">
+        <v>0.92212611949454004</v>
+      </c>
+      <c r="G47" s="12">
+        <v>1</v>
+      </c>
+      <c r="H47" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L47" s="27"/>
+      <c r="Q47" s="27"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="11"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C48" s="28">
+        <v>0.59065144628566402</v>
+      </c>
+      <c r="D48" s="12">
+        <v>0</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F48" s="28">
+        <v>0.87495852557437104</v>
+      </c>
+      <c r="G48" s="12">
+        <v>0.84</v>
+      </c>
+      <c r="H48" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L48" s="27"/>
+      <c r="Q48" s="27"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="11"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C49" s="28">
+        <v>0.50945176199800402</v>
+      </c>
+      <c r="D49" s="12">
+        <v>0</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F49" s="28">
+        <v>0.77788618990007097</v>
+      </c>
+      <c r="G49" s="12">
+        <v>0.64</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L49" s="27"/>
+      <c r="Q49" s="27"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="11"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C50" s="28">
+        <v>0.59723039365408503</v>
+      </c>
+      <c r="D50" s="12">
+        <v>0</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F50" s="28">
+        <v>0.830725488215312</v>
+      </c>
+      <c r="G50" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="H50" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L50" s="27"/>
+      <c r="Q50" s="27"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="11"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C51" s="28">
+        <v>0.57689781433924803</v>
+      </c>
+      <c r="D51" s="12">
+        <v>0</v>
+      </c>
+      <c r="E51" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F51" s="28">
+        <v>0.72865278715186899</v>
+      </c>
+      <c r="G51" s="12">
+        <v>0.53</v>
+      </c>
+      <c r="H51" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L51" s="27"/>
+      <c r="Q51" s="27"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="11"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C52" s="28">
+        <v>0.51808822206451799</v>
+      </c>
+      <c r="D52" s="12">
+        <v>0</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F52" s="28">
+        <v>0.68673806879667498</v>
+      </c>
+      <c r="G52" s="12">
+        <v>0.46</v>
+      </c>
+      <c r="H52" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L52" s="27"/>
+      <c r="Q52" s="27"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="11"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C53" s="28">
+        <v>0.62662191676512602</v>
+      </c>
+      <c r="D53" s="12">
+        <v>0</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F53" s="28">
+        <v>0.90176479044211499</v>
+      </c>
+      <c r="G53" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="H53" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="L53" s="27"/>
+      <c r="Q53" s="27"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="11"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C54" s="28">
+        <v>0.540283764367816</v>
+      </c>
+      <c r="D54" s="12">
+        <v>0</v>
+      </c>
+      <c r="E54" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F54" s="28">
+        <v>0.77835295092838197</v>
+      </c>
+      <c r="G54" s="12">
+        <v>0.62</v>
+      </c>
+      <c r="H54" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L54" s="27"/>
+      <c r="Q54" s="27"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="11"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C55" s="28">
+        <v>0.95061450956518301</v>
+      </c>
+      <c r="D55" s="12">
+        <v>0.37</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F55" s="28">
+        <v>0.77357994487326898</v>
+      </c>
+      <c r="G55" s="12">
+        <v>0.37</v>
+      </c>
+      <c r="H55" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L55" s="27"/>
+      <c r="Q55" s="27"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="11"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C56" s="28">
+        <v>0.96179003816291597</v>
+      </c>
+      <c r="D56" s="12">
+        <v>1</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F56" s="28">
+        <v>0.91918101671965102</v>
+      </c>
+      <c r="G56" s="12">
+        <v>1</v>
+      </c>
+      <c r="H56" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L56" s="27"/>
+      <c r="Q56" s="27"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="11"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C57" s="28">
+        <v>0.62382027828480402</v>
+      </c>
+      <c r="D57" s="12">
+        <v>0.66</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F57" s="28">
+        <v>0.91620295099302695</v>
+      </c>
+      <c r="G57" s="12">
+        <v>0.91</v>
+      </c>
+      <c r="H57" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L57" s="27"/>
+      <c r="Q57" s="27"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="11"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C58" s="28">
+        <v>0.58236805134817904</v>
+      </c>
+      <c r="D58" s="12">
+        <v>0</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F58" s="28">
+        <v>0.79565173527037902</v>
+      </c>
+      <c r="G58" s="12">
+        <v>0.63</v>
+      </c>
+      <c r="H58" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L58" s="27"/>
+      <c r="Q58" s="27"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="11"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C59" s="28">
+        <v>0.54738335224280199</v>
+      </c>
+      <c r="D59" s="12">
+        <v>0</v>
+      </c>
+      <c r="E59" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F59" s="28">
+        <v>0.58945278291835701</v>
+      </c>
+      <c r="G59" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="H59" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L59" s="27"/>
+      <c r="Q59" s="27"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="11"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C60" s="28">
+        <v>0.613414089443997</v>
+      </c>
+      <c r="D60" s="12">
+        <v>0</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F60" s="28">
+        <v>0.84722369815929299</v>
+      </c>
+      <c r="G60" s="12">
+        <v>0.66</v>
+      </c>
+      <c r="H60" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L60" s="27"/>
+      <c r="Q60" s="27"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="11"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C61" s="28">
+        <v>0.96471036273667798</v>
+      </c>
+      <c r="D61" s="12">
+        <v>1</v>
+      </c>
+      <c r="E61" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F61" s="28">
+        <v>0.87913392610973196</v>
+      </c>
+      <c r="G61" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="H61" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L61" s="27"/>
+      <c r="Q61" s="27"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="11"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C62" s="28">
+        <v>0.96587078651685299</v>
+      </c>
+      <c r="D62" s="12">
+        <v>1</v>
+      </c>
+      <c r="E62" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F62" s="28">
+        <v>0.93719972878729096</v>
+      </c>
+      <c r="G62" s="12">
+        <v>1</v>
+      </c>
+      <c r="H62" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L62" s="27"/>
+      <c r="Q62" s="27"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="11"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C63" s="28">
+        <v>0.56600235005562605</v>
+      </c>
+      <c r="D63" s="12">
+        <v>0</v>
+      </c>
+      <c r="E63" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F63" s="28">
+        <v>0.94297167544759997</v>
+      </c>
+      <c r="G63" s="12">
+        <v>0.81</v>
+      </c>
+      <c r="H63" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="L63" s="27"/>
+      <c r="Q63" s="27"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="9"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="11"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C64" s="28">
+        <v>0.96395524118738396</v>
+      </c>
+      <c r="D64" s="12">
+        <v>1</v>
+      </c>
+      <c r="E64" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F64" s="28">
+        <v>0.93281074019011501</v>
+      </c>
+      <c r="G64" s="35">
+        <v>1</v>
+      </c>
+      <c r="H64" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L64" s="27"/>
+      <c r="Q64" s="27"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="9"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="11"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C65" s="28">
+        <v>0.56295034373838704</v>
+      </c>
+      <c r="D65" s="12">
+        <v>0</v>
+      </c>
+      <c r="E65" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F65" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G65" s="14">
+        <v>0</v>
+      </c>
+      <c r="H65" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="L65" s="27"/>
+      <c r="Q65" s="27"/>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="11"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C66" s="28">
+        <v>0.64319409916220305</v>
+      </c>
+      <c r="D66" s="12">
+        <v>0</v>
+      </c>
+      <c r="E66" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F66" s="28">
+        <v>0.91622531696005405</v>
+      </c>
+      <c r="G66" s="12">
+        <v>1</v>
+      </c>
+      <c r="H66" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L66" s="27"/>
+      <c r="Q66" s="27"/>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="11"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C67" s="28">
+        <v>0.58865414106041303</v>
+      </c>
+      <c r="D67" s="12">
+        <v>0</v>
+      </c>
+      <c r="E67" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F67" s="28">
+        <v>0.91853992858859401</v>
+      </c>
+      <c r="G67" s="12">
+        <v>1</v>
+      </c>
+      <c r="H67" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L67" s="27"/>
+      <c r="Q67" s="27"/>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C68" s="9"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="11"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C68" s="28">
+        <v>0.96687177901463595</v>
+      </c>
+      <c r="D68" s="12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E68" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F68" s="28">
+        <v>0.952581458719851</v>
+      </c>
+      <c r="G68" s="12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H68" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="L68" s="27"/>
+      <c r="Q68" s="27"/>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C69" s="9"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="11"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C69" s="28">
+        <v>0.96708037825059101</v>
+      </c>
+      <c r="D69" s="12">
+        <v>0.91</v>
+      </c>
+      <c r="E69" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F69" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G69" s="14">
+        <v>0</v>
+      </c>
+      <c r="H69" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="L69" s="27"/>
+      <c r="Q69" s="27"/>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="9"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="11"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C70" s="28">
+        <v>0.92014851932405695</v>
+      </c>
+      <c r="D70" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="E70" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F70" s="28">
+        <v>0.87629814215635105</v>
+      </c>
+      <c r="G70" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="H70" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L70" s="27"/>
+      <c r="Q70" s="27"/>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="9"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="11"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C71" s="28">
+        <v>0.91748796718940595</v>
+      </c>
+      <c r="D71" s="12">
+        <v>0.76</v>
+      </c>
+      <c r="E71" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F71" s="28">
+        <v>0.85568917498983099</v>
+      </c>
+      <c r="G71" s="12">
+        <v>0.76</v>
+      </c>
+      <c r="H71" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="L71" s="27"/>
+      <c r="Q71" s="27"/>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C72" s="9"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="11"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C72" s="28">
+        <v>0.64018160719138595</v>
+      </c>
+      <c r="D72" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="E72" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F72" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G72" s="14">
+        <v>0</v>
+      </c>
+      <c r="H72" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="L72" s="27"/>
+      <c r="Q72" s="27"/>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="11"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C73" s="28">
+        <v>0.969948107448107</v>
+      </c>
+      <c r="D73" s="12">
+        <v>1</v>
+      </c>
+      <c r="E73" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F73" s="28">
+        <v>0.93100368898241204</v>
+      </c>
+      <c r="G73" s="12">
+        <v>1</v>
+      </c>
+      <c r="H73" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L73" s="27"/>
+      <c r="Q73" s="27"/>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C74" s="9"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="11"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C74" s="28">
+        <v>0.604589291030322</v>
+      </c>
+      <c r="D74" s="12">
+        <v>0</v>
+      </c>
+      <c r="E74" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F74" s="28">
+        <v>0.95551286856571704</v>
+      </c>
+      <c r="G74" s="12">
+        <v>1</v>
+      </c>
+      <c r="H74" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L74" s="27"/>
+      <c r="Q74" s="27"/>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C75" s="9"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="11"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C75" s="28">
+        <v>0.59006538749431003</v>
+      </c>
+      <c r="D75" s="12">
+        <v>0</v>
+      </c>
+      <c r="E75" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F75" s="28">
+        <v>0.55842336885836696</v>
+      </c>
+      <c r="G75" s="12">
+        <v>0</v>
+      </c>
+      <c r="H75" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L75" s="27"/>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="9"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="11"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C76" s="28">
+        <v>0.97213140262878495</v>
+      </c>
+      <c r="D76" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="E76" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F76" s="28">
+        <v>0.85111630729901</v>
+      </c>
+      <c r="G76" s="12">
+        <v>0.63</v>
+      </c>
+      <c r="H76" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L76" s="27"/>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C77" s="9"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="11"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C77" s="28">
+        <v>0.95960915219082099</v>
+      </c>
+      <c r="D77" s="12">
+        <v>1</v>
+      </c>
+      <c r="E77" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F77" s="28">
+        <v>0.91836271713767104</v>
+      </c>
+      <c r="G77" s="12">
+        <v>1</v>
+      </c>
+      <c r="H77" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L77" s="27"/>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C78" s="9"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="11"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C78" s="28">
+        <v>0.571755479965112</v>
+      </c>
+      <c r="D78" s="12">
+        <v>0</v>
+      </c>
+      <c r="E78" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F78" s="28">
+        <v>0.79161568205070199</v>
+      </c>
+      <c r="G78" s="12">
+        <v>0.72</v>
+      </c>
+      <c r="H78" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L78" s="27"/>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C79" s="9"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="11"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C79" s="28">
+        <v>0.57362921074056095</v>
+      </c>
+      <c r="D79" s="12">
+        <v>0</v>
+      </c>
+      <c r="E79" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F79" s="28">
+        <v>0.67399613121756297</v>
+      </c>
+      <c r="G79" s="12">
+        <v>0.33</v>
+      </c>
+      <c r="H79" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L79" s="27"/>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C80" s="9"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="11"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C80" s="28">
+        <v>0.552634678525316</v>
+      </c>
+      <c r="D80" s="12">
+        <v>0</v>
+      </c>
+      <c r="E80" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F80" s="28">
+        <v>0.79474645581093095</v>
+      </c>
+      <c r="G80" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="H80" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L80" s="27"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C81" s="9"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="11"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C81" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D81" s="14">
+        <v>0</v>
+      </c>
+      <c r="E81" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="F81" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G81" s="14">
+        <v>0</v>
+      </c>
+      <c r="H81" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="L81" s="27"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C82" s="9"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="11"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C82" s="28">
+        <v>0.59787443295048803</v>
+      </c>
+      <c r="D82" s="12">
+        <v>0</v>
+      </c>
+      <c r="E82" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F82" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G82" s="30">
+        <v>0</v>
+      </c>
+      <c r="H82" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="L82" s="27"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C83" s="9"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="11"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C83" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D83" s="14">
+        <v>0</v>
+      </c>
+      <c r="E83" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="F83" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G83" s="14">
+        <v>0</v>
+      </c>
+      <c r="H83" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="L83" s="27"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C84" s="9"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="11"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C84" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D84" s="14">
+        <v>0</v>
+      </c>
+      <c r="E84" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="F84" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G84" s="14">
+        <v>0</v>
+      </c>
+      <c r="H84" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="L84" s="27"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C85" s="9"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="11"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C85" s="28">
+        <v>0.54068211736349003</v>
+      </c>
+      <c r="D85" s="12">
+        <v>0</v>
+      </c>
+      <c r="E85" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F85" s="28">
+        <v>0.64369596100923498</v>
+      </c>
+      <c r="G85" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H85" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C86" s="21">
+      <c r="C86" s="19">
         <v>0.95735076327181501</v>
       </c>
-      <c r="D86" s="23">
+      <c r="D86" s="20">
         <v>1</v>
       </c>
-      <c r="E86" s="22" t="s">
+      <c r="E86" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="F86" s="23">
+      <c r="F86" s="20">
         <v>0.93107890616289202</v>
       </c>
-      <c r="G86" s="23">
+      <c r="G86" s="20">
         <v>1</v>
       </c>
-      <c r="H86" s="22" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H86" s="34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C87" s="16">
+      <c r="C87" s="14">
         <v>0.63893105889245005</v>
       </c>
-      <c r="D87" s="16">
-        <v>0</v>
-      </c>
-      <c r="E87" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F87" s="16">
+      <c r="D87" s="14">
+        <v>0</v>
+      </c>
+      <c r="E87" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F87" s="14">
         <v>0.92337132003798605</v>
       </c>
-      <c r="G87" s="16">
+      <c r="G87" s="14">
         <v>1</v>
       </c>
-      <c r="H87" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H87" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C88" s="16">
+      <c r="C88" s="14">
         <v>0.51995964974114794</v>
       </c>
-      <c r="D88" s="16">
-        <v>0</v>
-      </c>
-      <c r="E88" s="17" t="s">
+      <c r="D88" s="14">
+        <v>0</v>
+      </c>
+      <c r="E88" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="F88" s="16">
+      <c r="F88" s="14">
         <v>0.70611881788273401</v>
       </c>
-      <c r="G88" s="16">
+      <c r="G88" s="14">
         <v>0.36</v>
       </c>
-      <c r="H88" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H88" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C89" s="16">
+      <c r="C89" s="14">
         <v>0.64468912943277701</v>
       </c>
-      <c r="D89" s="16">
-        <v>0</v>
-      </c>
-      <c r="E89" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F89" s="16">
+      <c r="D89" s="14">
+        <v>0</v>
+      </c>
+      <c r="E89" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F89" s="14">
         <v>0.91068007662835204</v>
       </c>
-      <c r="G89" s="16">
+      <c r="G89" s="14">
         <v>0.8</v>
       </c>
-      <c r="H89" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H89" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C90" s="16">
+      <c r="C90" s="14">
         <v>0.56578415811865002</v>
       </c>
-      <c r="D90" s="16">
-        <v>0</v>
-      </c>
-      <c r="E90" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F90" s="16">
+      <c r="D90" s="14">
+        <v>0</v>
+      </c>
+      <c r="E90" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F90" s="14">
         <v>0.92797252370166905</v>
       </c>
-      <c r="G90" s="16">
+      <c r="G90" s="14">
         <v>0.92</v>
       </c>
-      <c r="H90" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H90" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C91" s="16">
+      <c r="C91" s="14">
         <v>0.51808822206451799</v>
       </c>
-      <c r="D91" s="16">
-        <v>0</v>
-      </c>
-      <c r="E91" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F91" s="16">
+      <c r="D91" s="14">
+        <v>0</v>
+      </c>
+      <c r="E91" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F91" s="14">
         <v>0.63547743441347004</v>
       </c>
-      <c r="G91" s="16">
+      <c r="G91" s="14">
         <v>0.3</v>
       </c>
-      <c r="H91" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H91" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C92" s="18" t="s">
+      <c r="C92" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D92" s="16">
-        <v>0</v>
-      </c>
-      <c r="E92" s="17" t="s">
+      <c r="D92" s="14">
+        <v>0</v>
+      </c>
+      <c r="E92" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="F92" s="16" t="s">
+      <c r="F92" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G92" s="16">
-        <v>0</v>
-      </c>
-      <c r="H92" s="17" t="s">
+      <c r="G92" s="14">
+        <v>0</v>
+      </c>
+      <c r="H92" s="31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C93" s="16">
+      <c r="C93" s="14">
         <v>0.60795795439192002</v>
       </c>
-      <c r="D93" s="16">
-        <v>0</v>
-      </c>
-      <c r="E93" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F93" s="16">
+      <c r="D93" s="14">
+        <v>0</v>
+      </c>
+      <c r="E93" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F93" s="14">
         <v>0.92110105158959699</v>
       </c>
-      <c r="G93" s="16">
+      <c r="G93" s="14">
         <v>1</v>
       </c>
-      <c r="H93" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H93" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C94" s="16">
+      <c r="C94" s="14">
         <v>0.604589291030322</v>
       </c>
-      <c r="D94" s="16">
-        <v>0</v>
-      </c>
-      <c r="E94" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F94" s="16">
+      <c r="D94" s="14">
+        <v>0</v>
+      </c>
+      <c r="E94" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F94" s="14">
         <v>0.95551286856571704</v>
       </c>
-      <c r="G94" s="16">
+      <c r="G94" s="14">
         <v>1</v>
       </c>
-      <c r="H94" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H94" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C95" s="16">
+      <c r="C95" s="14">
         <v>0.63550433996308398</v>
       </c>
-      <c r="D95" s="16">
-        <v>0</v>
-      </c>
-      <c r="E95" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F95" s="16">
+      <c r="D95" s="14">
+        <v>0</v>
+      </c>
+      <c r="E95" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F95" s="14">
         <v>0.91166883426896905</v>
       </c>
-      <c r="G95" s="16">
+      <c r="G95" s="14">
         <v>0.77</v>
       </c>
-      <c r="H95" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H95" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C96" s="16">
+      <c r="C96" s="14">
         <v>0.62115721888716302</v>
       </c>
-      <c r="D96" s="16">
-        <v>0</v>
-      </c>
-      <c r="E96" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F96" s="16">
+      <c r="D96" s="14">
+        <v>0</v>
+      </c>
+      <c r="E96" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F96" s="14">
         <v>0.89886403919977198</v>
       </c>
-      <c r="G96" s="16">
+      <c r="G96" s="14">
         <v>0.77</v>
       </c>
-      <c r="H96" s="17" t="s">
+      <c r="H96" s="31" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2589,22 +3349,22 @@
       <c r="B97" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C97" s="16">
+      <c r="C97" s="14">
         <v>0.60528629931956102</v>
       </c>
-      <c r="D97" s="16">
-        <v>0</v>
-      </c>
-      <c r="E97" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F97" s="16">
+      <c r="D97" s="14">
+        <v>0</v>
+      </c>
+      <c r="E97" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F97" s="14">
         <v>0.90092381440125002</v>
       </c>
-      <c r="G97" s="16">
+      <c r="G97" s="14">
         <v>0.77</v>
       </c>
-      <c r="H97" s="17" t="s">
+      <c r="H97" s="31" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2615,22 +3375,22 @@
       <c r="B98" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C98" s="16">
+      <c r="C98" s="14">
         <v>0.53597944754065296</v>
       </c>
-      <c r="D98" s="16">
-        <v>0</v>
-      </c>
-      <c r="E98" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F98" s="16">
+      <c r="D98" s="14">
+        <v>0</v>
+      </c>
+      <c r="E98" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F98" s="14">
         <v>0.75762205138313898</v>
       </c>
-      <c r="G98" s="16">
+      <c r="G98" s="14">
         <v>0.3</v>
       </c>
-      <c r="H98" s="17" t="s">
+      <c r="H98" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2641,22 +3401,22 @@
       <c r="B99" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C99" s="16">
+      <c r="C99" s="14">
         <v>0.56330647505100095</v>
       </c>
-      <c r="D99" s="16">
-        <v>0</v>
-      </c>
-      <c r="E99" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F99" s="16">
+      <c r="D99" s="14">
+        <v>0</v>
+      </c>
+      <c r="E99" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F99" s="14">
         <v>0.85686118313866</v>
       </c>
-      <c r="G99" s="16">
+      <c r="G99" s="14">
         <v>0.6</v>
       </c>
-      <c r="H99" s="17" t="s">
+      <c r="H99" s="15" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2667,22 +3427,22 @@
       <c r="B100" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C100" s="16">
+      <c r="C100" s="14">
         <v>0.60156226777291399</v>
       </c>
-      <c r="D100" s="16">
-        <v>0</v>
-      </c>
-      <c r="E100" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F100" s="16">
+      <c r="D100" s="14">
+        <v>0</v>
+      </c>
+      <c r="E100" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F100" s="14">
         <v>0.91157639199198304</v>
       </c>
-      <c r="G100" s="16">
+      <c r="G100" s="14">
         <v>0.88</v>
       </c>
-      <c r="H100" s="17" t="s">
+      <c r="H100" s="15" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2693,22 +3453,22 @@
       <c r="B101" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C101" s="16">
+      <c r="C101" s="14">
         <v>0.66324371677235106</v>
       </c>
-      <c r="D101" s="16">
-        <v>0</v>
-      </c>
-      <c r="E101" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F101" s="16">
+      <c r="D101" s="14">
+        <v>0</v>
+      </c>
+      <c r="E101" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F101" s="14">
         <v>0.80372865972307495</v>
       </c>
-      <c r="G101" s="16">
+      <c r="G101" s="14">
         <v>0.81</v>
       </c>
-      <c r="H101" s="17" t="s">
+      <c r="H101" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2719,22 +3479,22 @@
       <c r="B102" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C102" s="16">
+      <c r="C102" s="14">
         <v>0.56625368310739799</v>
       </c>
-      <c r="D102" s="16">
-        <v>0</v>
-      </c>
-      <c r="E102" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F102" s="16">
+      <c r="D102" s="14">
+        <v>0</v>
+      </c>
+      <c r="E102" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F102" s="14">
         <v>0.93939437755227195</v>
       </c>
-      <c r="G102" s="16">
+      <c r="G102" s="14">
         <v>1</v>
       </c>
-      <c r="H102" s="17" t="s">
+      <c r="H102" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2745,22 +3505,22 @@
       <c r="B103" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C103" s="16">
+      <c r="C103" s="14">
         <v>0.96622581148564302</v>
       </c>
-      <c r="D103" s="16">
+      <c r="D103" s="14">
         <v>0.9</v>
       </c>
-      <c r="E103" s="17" t="s">
+      <c r="E103" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="F103" s="16">
+      <c r="F103" s="14">
         <v>0.92638170870188796</v>
       </c>
-      <c r="G103" s="16">
+      <c r="G103" s="14">
         <v>1</v>
       </c>
-      <c r="H103" s="17" t="s">
+      <c r="H103" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2771,22 +3531,22 @@
       <c r="B104" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C104" s="16">
+      <c r="C104" s="14">
         <v>0.72199943092609697</v>
       </c>
-      <c r="D104" s="16">
-        <v>0</v>
-      </c>
-      <c r="E104" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F104" s="16">
+      <c r="D104" s="14">
+        <v>0</v>
+      </c>
+      <c r="E104" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F104" s="14">
         <v>0.80207845826754298</v>
       </c>
-      <c r="G104" s="16">
+      <c r="G104" s="14">
         <v>0.46</v>
       </c>
-      <c r="H104" s="17" t="s">
+      <c r="H104" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2797,22 +3557,22 @@
       <c r="B105" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C105" s="16">
+      <c r="C105" s="14">
         <v>0.59723039365408503</v>
       </c>
-      <c r="D105" s="16">
-        <v>0</v>
-      </c>
-      <c r="E105" s="17" t="s">
+      <c r="D105" s="14">
+        <v>0</v>
+      </c>
+      <c r="E105" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="F105" s="16">
+      <c r="F105" s="14">
         <v>0.80961264700742597</v>
       </c>
-      <c r="G105" s="16">
+      <c r="G105" s="14">
         <v>0.69</v>
       </c>
-      <c r="H105" s="17" t="s">
+      <c r="H105" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2823,22 +3583,22 @@
       <c r="B106" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C106" s="16">
+      <c r="C106" s="14">
         <v>0.59522404863465095</v>
       </c>
-      <c r="D106" s="16">
-        <v>0</v>
-      </c>
-      <c r="E106" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F106" s="16">
+      <c r="D106" s="14">
+        <v>0</v>
+      </c>
+      <c r="E106" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F106" s="14">
         <v>0.60401473146264095</v>
       </c>
-      <c r="G106" s="16">
+      <c r="G106" s="14">
         <v>0.11</v>
       </c>
-      <c r="H106" s="17" t="s">
+      <c r="H106" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2849,22 +3609,22 @@
       <c r="B107" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C107" s="16">
+      <c r="C107" s="14">
         <v>0.46043053803766398</v>
       </c>
-      <c r="D107" s="16">
-        <v>0</v>
-      </c>
-      <c r="E107" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F107" s="16">
+      <c r="D107" s="14">
+        <v>0</v>
+      </c>
+      <c r="E107" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F107" s="14">
         <v>0.64320471889860398</v>
       </c>
-      <c r="G107" s="16">
+      <c r="G107" s="14">
         <v>0.32</v>
       </c>
-      <c r="H107" s="17" t="s">
+      <c r="H107" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2875,22 +3635,22 @@
       <c r="B108" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C108" s="16">
+      <c r="C108" s="14">
         <v>0.54358330804825805</v>
       </c>
-      <c r="D108" s="16">
-        <v>0</v>
-      </c>
-      <c r="E108" s="17" t="s">
+      <c r="D108" s="14">
+        <v>0</v>
+      </c>
+      <c r="E108" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="F108" s="16">
+      <c r="F108" s="14">
         <v>0.75517343210782495</v>
       </c>
-      <c r="G108" s="16">
+      <c r="G108" s="14">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H108" s="17" t="s">
+      <c r="H108" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2901,22 +3661,22 @@
       <c r="B109" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C109" s="16">
+      <c r="C109" s="14">
         <v>0.55960071701506198</v>
       </c>
-      <c r="D109" s="16">
-        <v>0</v>
-      </c>
-      <c r="E109" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F109" s="16">
+      <c r="D109" s="14">
+        <v>0</v>
+      </c>
+      <c r="E109" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F109" s="14">
         <v>0.80903193388792405</v>
       </c>
-      <c r="G109" s="16">
+      <c r="G109" s="14">
         <v>0.52</v>
       </c>
-      <c r="H109" s="17" t="s">
+      <c r="H109" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2927,22 +3687,22 @@
       <c r="B110" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C110" s="16">
+      <c r="C110" s="14">
         <v>0.42762224536486898</v>
       </c>
-      <c r="D110" s="16">
-        <v>0</v>
-      </c>
-      <c r="E110" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F110" s="16">
+      <c r="D110" s="14">
+        <v>0</v>
+      </c>
+      <c r="E110" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F110" s="14">
         <v>0.67701277319617703</v>
       </c>
-      <c r="G110" s="16">
+      <c r="G110" s="14">
         <v>0.41</v>
       </c>
-      <c r="H110" s="17" t="s">
+      <c r="H110" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2953,22 +3713,22 @@
       <c r="B111" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C111" s="16">
+      <c r="C111" s="14">
         <v>0.47304523178475499</v>
       </c>
-      <c r="D111" s="16">
-        <v>0</v>
-      </c>
-      <c r="E111" s="17" t="s">
+      <c r="D111" s="14">
+        <v>0</v>
+      </c>
+      <c r="E111" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="F111" s="16">
+      <c r="F111" s="14">
         <v>0.53008492886153402</v>
       </c>
-      <c r="G111" s="16">
+      <c r="G111" s="14">
         <v>0.21</v>
       </c>
-      <c r="H111" s="17" t="s">
+      <c r="H111" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2979,22 +3739,22 @@
       <c r="B112" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C112" s="16">
+      <c r="C112" s="14">
         <v>0.53931072692026105</v>
       </c>
-      <c r="D112" s="16">
-        <v>0</v>
-      </c>
-      <c r="E112" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F112" s="16">
+      <c r="D112" s="14">
+        <v>0</v>
+      </c>
+      <c r="E112" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F112" s="14">
         <v>0.86022258570315202</v>
       </c>
-      <c r="G112" s="16">
+      <c r="G112" s="14">
         <v>0.33</v>
       </c>
-      <c r="H112" s="17" t="s">
+      <c r="H112" s="15" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3005,22 +3765,22 @@
       <c r="B113" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C113" s="16">
+      <c r="C113" s="14">
         <v>0.45807663194308201</v>
       </c>
-      <c r="D113" s="16">
-        <v>0</v>
-      </c>
-      <c r="E113" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F113" s="16">
+      <c r="D113" s="14">
+        <v>0</v>
+      </c>
+      <c r="E113" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F113" s="14">
         <v>0.474512904142391</v>
       </c>
-      <c r="G113" s="16">
+      <c r="G113" s="14">
         <v>0.03</v>
       </c>
-      <c r="H113" s="17" t="s">
+      <c r="H113" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3031,22 +3791,22 @@
       <c r="B114" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C114" s="16">
+      <c r="C114" s="14">
         <v>0.52632391393324596</v>
       </c>
-      <c r="D114" s="16">
-        <v>0</v>
-      </c>
-      <c r="E114" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F114" s="16">
+      <c r="D114" s="14">
+        <v>0</v>
+      </c>
+      <c r="E114" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F114" s="14">
         <v>0.85207423651353498</v>
       </c>
-      <c r="G114" s="16">
+      <c r="G114" s="14">
         <v>0.78</v>
       </c>
-      <c r="H114" s="17" t="s">
+      <c r="H114" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3057,22 +3817,22 @@
       <c r="B115" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C115" s="16">
+      <c r="C115" s="14">
         <v>0.57772448970287504</v>
       </c>
-      <c r="D115" s="16">
-        <v>0</v>
-      </c>
-      <c r="E115" s="17" t="s">
+      <c r="D115" s="14">
+        <v>0</v>
+      </c>
+      <c r="E115" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="F115" s="16">
+      <c r="F115" s="14">
         <v>0.76722006719806002</v>
       </c>
-      <c r="G115" s="16">
+      <c r="G115" s="14">
         <v>0.54</v>
       </c>
-      <c r="H115" s="17" t="s">
+      <c r="H115" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3083,22 +3843,22 @@
       <c r="B116" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C116" s="16">
+      <c r="C116" s="14">
         <v>0.553124797171199</v>
       </c>
-      <c r="D116" s="16">
-        <v>0</v>
-      </c>
-      <c r="E116" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F116" s="16">
+      <c r="D116" s="14">
+        <v>0</v>
+      </c>
+      <c r="E116" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F116" s="14">
         <v>0.73929132964798805</v>
       </c>
-      <c r="G116" s="16">
+      <c r="G116" s="14">
         <v>0.42</v>
       </c>
-      <c r="H116" s="17" t="s">
+      <c r="H116" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3109,22 +3869,22 @@
       <c r="B117" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C117" s="16">
+      <c r="C117" s="14">
         <v>0.56896731239943099</v>
       </c>
-      <c r="D117" s="16">
-        <v>0</v>
-      </c>
-      <c r="E117" s="17" t="s">
+      <c r="D117" s="14">
+        <v>0</v>
+      </c>
+      <c r="E117" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="F117" s="16">
+      <c r="F117" s="14">
         <v>0.76488220676096597</v>
       </c>
-      <c r="G117" s="16">
+      <c r="G117" s="14">
         <v>0.51</v>
       </c>
-      <c r="H117" s="17" t="s">
+      <c r="H117" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3135,22 +3895,22 @@
       <c r="B118" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C118" s="16">
+      <c r="C118" s="14">
         <v>0.53476818628215095</v>
       </c>
-      <c r="D118" s="16">
-        <v>0</v>
-      </c>
-      <c r="E118" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F118" s="16">
+      <c r="D118" s="14">
+        <v>0</v>
+      </c>
+      <c r="E118" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F118" s="14">
         <v>0.54469942551697303</v>
       </c>
-      <c r="G118" s="16">
+      <c r="G118" s="14">
         <v>0.02</v>
       </c>
-      <c r="H118" s="17" t="s">
+      <c r="H118" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3161,22 +3921,22 @@
       <c r="B119" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C119" s="16">
+      <c r="C119" s="14">
         <v>0.61894795845087003</v>
       </c>
-      <c r="D119" s="16">
-        <v>0</v>
-      </c>
-      <c r="E119" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F119" s="16">
+      <c r="D119" s="14">
+        <v>0</v>
+      </c>
+      <c r="E119" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F119" s="14">
         <v>0.91778104339033495</v>
       </c>
-      <c r="G119" s="16">
+      <c r="G119" s="14">
         <v>1</v>
       </c>
-      <c r="H119" s="17" t="s">
+      <c r="H119" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3187,22 +3947,22 @@
       <c r="B120" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C120" s="16">
+      <c r="C120" s="14">
         <v>0.88889943969212604</v>
       </c>
-      <c r="D120" s="16">
+      <c r="D120" s="14">
         <v>0.84</v>
       </c>
-      <c r="E120" s="17" t="s">
+      <c r="E120" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="F120" s="16">
+      <c r="F120" s="14">
         <v>0.84140001058622005</v>
       </c>
-      <c r="G120" s="16">
+      <c r="G120" s="14">
         <v>0.84</v>
       </c>
-      <c r="H120" s="17" t="s">
+      <c r="H120" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3213,22 +3973,22 @@
       <c r="B121" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C121" s="16">
+      <c r="C121" s="14">
         <v>0.62614572346609298</v>
       </c>
-      <c r="D121" s="16">
-        <v>0</v>
-      </c>
-      <c r="E121" s="17" t="s">
+      <c r="D121" s="14">
+        <v>0</v>
+      </c>
+      <c r="E121" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="F121" s="16">
+      <c r="F121" s="14">
         <v>0.79620598057615699</v>
       </c>
-      <c r="G121" s="16">
+      <c r="G121" s="14">
         <v>0.53</v>
       </c>
-      <c r="H121" s="17" t="s">
+      <c r="H121" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3239,22 +3999,22 @@
       <c r="B122" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C122" s="16">
+      <c r="C122" s="14">
         <v>0.61113545845087003</v>
       </c>
-      <c r="D122" s="16">
-        <v>0</v>
-      </c>
-      <c r="E122" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F122" s="16">
+      <c r="D122" s="14">
+        <v>0</v>
+      </c>
+      <c r="E122" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F122" s="14">
         <v>0.91778104339033495</v>
       </c>
-      <c r="G122" s="16">
+      <c r="G122" s="14">
         <v>1</v>
       </c>
-      <c r="H122" s="17" t="s">
+      <c r="H122" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3265,22 +4025,22 @@
       <c r="B123" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C123" s="16">
+      <c r="C123" s="14">
         <v>0.56526412624391698</v>
       </c>
-      <c r="D123" s="16">
-        <v>0</v>
-      </c>
-      <c r="E123" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F123" s="16">
+      <c r="D123" s="14">
+        <v>0</v>
+      </c>
+      <c r="E123" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F123" s="14">
         <v>0.69249673503244102</v>
       </c>
-      <c r="G123" s="16">
+      <c r="G123" s="14">
         <v>0.3</v>
       </c>
-      <c r="H123" s="17" t="s">
+      <c r="H123" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3291,22 +4051,22 @@
       <c r="B124" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C124" s="18" t="s">
+      <c r="C124" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D124" s="16">
-        <v>0</v>
-      </c>
-      <c r="E124" s="17" t="s">
+      <c r="D124" s="14">
+        <v>0</v>
+      </c>
+      <c r="E124" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="F124" s="16" t="s">
+      <c r="F124" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G124" s="16">
-        <v>0</v>
-      </c>
-      <c r="H124" s="17" t="s">
+      <c r="G124" s="14">
+        <v>0</v>
+      </c>
+      <c r="H124" s="15" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3317,22 +4077,22 @@
       <c r="B125" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C125" s="16">
+      <c r="C125" s="14">
         <v>0.77508351526693897</v>
       </c>
-      <c r="D125" s="16">
+      <c r="D125" s="14">
         <v>0.33</v>
       </c>
-      <c r="E125" s="17" t="s">
+      <c r="E125" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="F125" s="16" t="s">
+      <c r="F125" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G125" s="16">
-        <v>0</v>
-      </c>
-      <c r="H125" s="17" t="s">
+      <c r="G125" s="14">
+        <v>0</v>
+      </c>
+      <c r="H125" s="15" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3343,22 +4103,22 @@
       <c r="B126" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C126" s="16">
+      <c r="C126" s="14">
         <v>0.55523818579279904</v>
       </c>
-      <c r="D126" s="16">
-        <v>0</v>
-      </c>
-      <c r="E126" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F126" s="16">
+      <c r="D126" s="14">
+        <v>0</v>
+      </c>
+      <c r="E126" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F126" s="14">
         <v>0.77158587719643901</v>
       </c>
-      <c r="G126" s="16">
+      <c r="G126" s="14">
         <v>0.5</v>
       </c>
-      <c r="H126" s="17" t="s">
+      <c r="H126" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3369,22 +4129,22 @@
       <c r="B127" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C127" s="16">
+      <c r="C127" s="14">
         <v>0.54780704203008601</v>
       </c>
-      <c r="D127" s="16">
-        <v>0</v>
-      </c>
-      <c r="E127" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F127" s="16">
+      <c r="D127" s="14">
+        <v>0</v>
+      </c>
+      <c r="E127" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F127" s="14">
         <v>0.78201778993948201</v>
       </c>
-      <c r="G127" s="16">
+      <c r="G127" s="14">
         <v>0.6</v>
       </c>
-      <c r="H127" s="17" t="s">
+      <c r="H127" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3395,22 +4155,22 @@
       <c r="B128" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C128" s="16">
+      <c r="C128" s="14">
         <v>0.96758966244725697</v>
       </c>
-      <c r="D128" s="16">
+      <c r="D128" s="14">
         <v>1</v>
       </c>
-      <c r="E128" s="17" t="s">
+      <c r="E128" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="F128" s="16">
+      <c r="F128" s="14">
         <v>0.93477757085247004</v>
       </c>
-      <c r="G128" s="16">
+      <c r="G128" s="14">
         <v>1</v>
       </c>
-      <c r="H128" s="17" t="s">
+      <c r="H128" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3421,22 +4181,22 @@
       <c r="B129" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C129" s="16">
+      <c r="C129" s="14">
         <v>0.95895395160042596</v>
       </c>
-      <c r="D129" s="16">
-        <v>0</v>
-      </c>
-      <c r="E129" s="17" t="s">
+      <c r="D129" s="14">
+        <v>0</v>
+      </c>
+      <c r="E129" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="F129" s="16">
+      <c r="F129" s="14">
         <v>0.90946492476243901</v>
       </c>
-      <c r="G129" s="16">
+      <c r="G129" s="14">
         <v>0.85</v>
       </c>
-      <c r="H129" s="17" t="s">
+      <c r="H129" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3447,22 +4207,22 @@
       <c r="B130" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C130" s="16">
+      <c r="C130" s="14">
         <v>0.97205956496686796</v>
       </c>
-      <c r="D130" s="16">
-        <v>0</v>
-      </c>
-      <c r="E130" s="17" t="s">
+      <c r="D130" s="14">
+        <v>0</v>
+      </c>
+      <c r="E130" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="F130" s="16">
+      <c r="F130" s="14">
         <v>0.92146884794356698</v>
       </c>
-      <c r="G130" s="16">
+      <c r="G130" s="14">
         <v>1</v>
       </c>
-      <c r="H130" s="17" t="s">
+      <c r="H130" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3473,22 +4233,22 @@
       <c r="B131" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C131" s="16">
+      <c r="C131" s="14">
         <v>0.95837684827170799</v>
       </c>
-      <c r="D131" s="16">
+      <c r="D131" s="14">
         <v>1</v>
       </c>
-      <c r="E131" s="17" t="s">
+      <c r="E131" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="F131" s="16">
+      <c r="F131" s="14">
         <v>0.92388934636511899</v>
       </c>
-      <c r="G131" s="16">
+      <c r="G131" s="14">
         <v>1</v>
       </c>
-      <c r="H131" s="17" t="s">
+      <c r="H131" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3499,22 +4259,22 @@
       <c r="B132" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C132" s="16">
+      <c r="C132" s="14">
         <v>0.776618624635806</v>
       </c>
-      <c r="D132" s="16">
+      <c r="D132" s="14">
         <v>0.27</v>
       </c>
-      <c r="E132" s="17" t="s">
+      <c r="E132" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="F132" s="16">
+      <c r="F132" s="14">
         <v>0.74608876180938599</v>
       </c>
-      <c r="G132" s="16">
+      <c r="G132" s="14">
         <v>0.27</v>
       </c>
-      <c r="H132" s="17" t="s">
+      <c r="H132" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3525,22 +4285,22 @@
       <c r="B133" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C133" s="16">
+      <c r="C133" s="14">
         <v>0.959365016319631</v>
       </c>
-      <c r="D133" s="16">
+      <c r="D133" s="14">
         <v>1</v>
       </c>
-      <c r="E133" s="17" t="s">
+      <c r="E133" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="F133" s="16">
+      <c r="F133" s="14">
         <v>0.93069815469086703</v>
       </c>
-      <c r="G133" s="16">
+      <c r="G133" s="14">
         <v>1</v>
       </c>
-      <c r="H133" s="17" t="s">
+      <c r="H133" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3551,22 +4311,22 @@
       <c r="B134" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C134" s="16">
+      <c r="C134" s="14">
         <v>0.68071127830311895</v>
       </c>
-      <c r="D134" s="16">
-        <v>0</v>
-      </c>
-      <c r="E134" s="17" t="s">
+      <c r="D134" s="14">
+        <v>0</v>
+      </c>
+      <c r="E134" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="F134" s="16">
+      <c r="F134" s="14">
         <v>0.91009419143276404</v>
       </c>
-      <c r="G134" s="16">
+      <c r="G134" s="14">
         <v>1</v>
       </c>
-      <c r="H134" s="17" t="s">
+      <c r="H134" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3577,22 +4337,22 @@
       <c r="B135" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C135" s="16">
+      <c r="C135" s="14">
         <v>0.96613773511056</v>
       </c>
-      <c r="D135" s="16">
-        <v>0</v>
-      </c>
-      <c r="E135" s="17" t="s">
+      <c r="D135" s="14">
+        <v>0</v>
+      </c>
+      <c r="E135" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="F135" s="16">
+      <c r="F135" s="14">
         <v>0.848920379820986</v>
       </c>
-      <c r="G135" s="16">
+      <c r="G135" s="14">
         <v>0.81</v>
       </c>
-      <c r="H135" s="17" t="s">
+      <c r="H135" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3603,22 +4363,22 @@
       <c r="B136" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C136" s="16">
+      <c r="C136" s="14">
         <v>0.50284780578898203</v>
       </c>
-      <c r="D136" s="16">
-        <v>0</v>
-      </c>
-      <c r="E136" s="17" t="s">
+      <c r="D136" s="14">
+        <v>0</v>
+      </c>
+      <c r="E136" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="F136" s="16">
+      <c r="F136" s="14">
         <v>0.65734889756427495</v>
       </c>
-      <c r="G136" s="16">
+      <c r="G136" s="14">
         <v>0.3</v>
       </c>
-      <c r="H136" s="17" t="s">
+      <c r="H136" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3629,22 +4389,22 @@
       <c r="B137" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C137" s="16">
+      <c r="C137" s="14">
         <v>0.47882971462819601</v>
       </c>
-      <c r="D137" s="16">
-        <v>0</v>
-      </c>
-      <c r="E137" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F137" s="16">
+      <c r="D137" s="14">
+        <v>0</v>
+      </c>
+      <c r="E137" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F137" s="14">
         <v>0.56739408859158202</v>
       </c>
-      <c r="G137" s="16">
+      <c r="G137" s="14">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H137" s="17" t="s">
+      <c r="H137" s="15" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3655,22 +4415,22 @@
       <c r="B138" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C138" s="18" t="s">
+      <c r="C138" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D138" s="16">
-        <v>0</v>
-      </c>
-      <c r="E138" s="17" t="s">
+      <c r="D138" s="14">
+        <v>0</v>
+      </c>
+      <c r="E138" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="F138" s="16" t="s">
+      <c r="F138" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G138" s="16">
-        <v>0</v>
-      </c>
-      <c r="H138" s="17" t="s">
+      <c r="G138" s="14">
+        <v>0</v>
+      </c>
+      <c r="H138" s="15" t="s">
         <v>149</v>
       </c>
     </row>

</xml_diff>